<commit_message>
Updated BOM on v1.6 Mini to use 820 ohm current limits rather than 330s.
</commit_message>
<xml_diff>
--- a/mini/v16/Fubarino_Mini_v16_BOM_SeeedFormat.xlsx
+++ b/mini/v16/Fubarino_Mini_v16_BOM_SeeedFormat.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\fubarino.github.com\mini\v16\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="24615" windowHeight="9135" tabRatio="795"/>
   </bookViews>
@@ -566,7 +561,7 @@
     <definedName name="美金對美金" localSheetId="0">#REF!</definedName>
     <definedName name="美金對美金">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -849,9 +844,6 @@
     <t>LED SMARTLED GREEN 570NM 0603</t>
   </si>
   <si>
-    <t>RES 330 OHM 1/10W 5% 0603 SMD</t>
-  </si>
-  <si>
     <t>RES 10K OHM 1/10W 5% 0603 SMD</t>
   </si>
   <si>
@@ -888,9 +880,6 @@
     <t>LG L29K-G2J1-24-Z</t>
   </si>
   <si>
-    <t>ERJ-3GEYJ331V</t>
-  </si>
-  <si>
     <t>ERJ-3GEYJ103V</t>
   </si>
   <si>
@@ -916,9 +905,6 @@
   </si>
   <si>
     <t>475-2709-1-ND</t>
-  </si>
-  <si>
-    <t>P330GCT-ND</t>
   </si>
   <si>
     <t>P10KGCT-ND</t>
@@ -982,9 +968,6 @@
   </si>
   <si>
     <t>GREEN</t>
-  </si>
-  <si>
-    <t>330 ohm</t>
   </si>
   <si>
     <t>10K ohm</t>
@@ -1085,6 +1068,18 @@
   <si>
     <t>Issue Date：03/14/2013</t>
   </si>
+  <si>
+    <t>RES 820 OHM 1/10W 5% 0603 SMD</t>
+  </si>
+  <si>
+    <t>820 ohm</t>
+  </si>
+  <si>
+    <t>ERJ-3GEYJ821V</t>
+  </si>
+  <si>
+    <t>P820GCT-ND</t>
+  </si>
 </sst>
 </file>
 
@@ -1122,7 +1117,7 @@
     <numFmt numFmtId="189" formatCode="\$#,##0;\(\$#,##0\)"/>
     <numFmt numFmtId="190" formatCode="#,##0;\(#,##0\)"/>
   </numFmts>
-  <fonts count="46">
+  <fonts count="47">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1394,6 +1389,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="14">
@@ -1979,7 +1980,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="348" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -2171,6 +2172,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="360" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="44" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="34" fillId="9" borderId="3" xfId="348" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -2183,15 +2193,8 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="362" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="366">
     <cellStyle name="_x001e_" xfId="1"/>
@@ -39263,7 +39266,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -39298,7 +39301,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -39512,10 +39515,10 @@
   </sheetPr>
   <dimension ref="A1:N77"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="13" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="13" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B19" sqref="B19"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="16.5"/>
@@ -39582,7 +39585,7 @@
     </row>
     <row r="6" spans="1:14" s="11" customFormat="1" ht="24.75" customHeight="1">
       <c r="A6" s="31" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B6" s="18"/>
       <c r="C6" s="16"/>
@@ -39594,7 +39597,7 @@
     </row>
     <row r="7" spans="1:14" s="11" customFormat="1" ht="24.75" customHeight="1">
       <c r="A7" s="19" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="16"/>
@@ -39606,7 +39609,7 @@
     </row>
     <row r="8" spans="1:14" s="11" customFormat="1" ht="24.75" customHeight="1">
       <c r="A8" s="46" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="17"/>
@@ -39627,98 +39630,98 @@
       <c r="N9" s="13"/>
     </row>
     <row r="10" spans="1:14" s="14" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A10" s="76" t="s">
+      <c r="A10" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="76" t="s">
+      <c r="B10" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="76" t="s">
+      <c r="C10" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="76" t="s">
+      <c r="D10" s="81" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="75" t="s">
+      <c r="E10" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="76" t="s">
+      <c r="F10" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="76" t="s">
+      <c r="G10" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="75" t="s">
+      <c r="H10" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="75" t="s">
+      <c r="I10" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="75" t="s">
+      <c r="J10" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="K10" s="75" t="s">
+      <c r="K10" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="L10" s="75" t="s">
+      <c r="L10" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="M10" s="75" t="s">
+      <c r="M10" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="N10" s="75" t="s">
+      <c r="N10" s="80" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="14" customFormat="1" ht="15" customHeight="1">
-      <c r="A11" s="76"/>
-      <c r="B11" s="76"/>
-      <c r="C11" s="76"/>
-      <c r="D11" s="76"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="76"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="75"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
-      <c r="L11" s="75"/>
-      <c r="M11" s="75"/>
-      <c r="N11" s="75"/>
+      <c r="A11" s="81"/>
+      <c r="B11" s="81"/>
+      <c r="C11" s="81"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="80"/>
+      <c r="I11" s="80"/>
+      <c r="J11" s="80"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="80"/>
+      <c r="M11" s="80"/>
+      <c r="N11" s="80"/>
     </row>
     <row r="12" spans="1:14" s="14" customFormat="1" ht="15" customHeight="1">
-      <c r="A12" s="76"/>
-      <c r="B12" s="76"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="76"/>
-      <c r="G12" s="76"/>
-      <c r="H12" s="75"/>
-      <c r="I12" s="75"/>
-      <c r="J12" s="75"/>
-      <c r="K12" s="75"/>
-      <c r="L12" s="75"/>
-      <c r="M12" s="75"/>
-      <c r="N12" s="75"/>
+      <c r="A12" s="81"/>
+      <c r="B12" s="81"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="80"/>
+      <c r="F12" s="81"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="80"/>
+      <c r="I12" s="80"/>
+      <c r="J12" s="80"/>
+      <c r="K12" s="80"/>
+      <c r="L12" s="80"/>
+      <c r="M12" s="80"/>
+      <c r="N12" s="80"/>
     </row>
     <row r="13" spans="1:14" s="12" customFormat="1" ht="21" customHeight="1">
-      <c r="A13" s="77" t="s">
+      <c r="A13" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="77"/>
-      <c r="C13" s="77"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="77"/>
-      <c r="F13" s="77"/>
-      <c r="G13" s="77"/>
-      <c r="H13" s="77"/>
-      <c r="I13" s="77"/>
-      <c r="J13" s="77"/>
-      <c r="K13" s="77"/>
-      <c r="L13" s="77"/>
-      <c r="M13" s="77"/>
-      <c r="N13" s="77"/>
+      <c r="B13" s="82"/>
+      <c r="C13" s="82"/>
+      <c r="D13" s="82"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="82"/>
+      <c r="G13" s="82"/>
+      <c r="H13" s="82"/>
+      <c r="I13" s="82"/>
+      <c r="J13" s="82"/>
+      <c r="K13" s="82"/>
+      <c r="L13" s="82"/>
+      <c r="M13" s="82"/>
+      <c r="N13" s="82"/>
     </row>
     <row r="14" spans="1:14" s="43" customFormat="1" ht="19.5" customHeight="1">
       <c r="A14" s="32" t="s">
@@ -39763,7 +39766,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="73" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C15" s="51">
         <v>1</v>
@@ -39778,19 +39781,19 @@
         <v>28</v>
       </c>
       <c r="G15" s="33" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H15" s="40" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I15" s="53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J15" s="54" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K15" s="55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L15" s="41"/>
       <c r="M15" s="41"/>
@@ -39801,7 +39804,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="73" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C16" s="51">
         <v>1</v>
@@ -39813,22 +39816,22 @@
         <v>47</v>
       </c>
       <c r="F16" s="33" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G16" s="33" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H16" s="40" t="s">
         <v>29</v>
       </c>
       <c r="I16" s="56" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J16" s="54" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K16" s="57" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L16" s="41"/>
       <c r="M16" s="41"/>
@@ -39839,7 +39842,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="73" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C17" s="51">
         <v>2</v>
@@ -39851,7 +39854,7 @@
         <v>48</v>
       </c>
       <c r="F17" s="33" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G17" s="33" t="s">
         <v>26</v>
@@ -39860,13 +39863,13 @@
         <v>29</v>
       </c>
       <c r="I17" s="53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J17" s="54" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K17" s="55" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L17" s="41"/>
       <c r="M17" s="41"/>
@@ -39883,26 +39886,26 @@
         <v>1</v>
       </c>
       <c r="D18" s="33" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E18" s="52" t="s">
         <v>49</v>
       </c>
       <c r="F18" s="33" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G18" s="33"/>
       <c r="H18" s="40" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="I18" s="59" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J18" s="54" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K18" s="60" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L18" s="34"/>
       <c r="M18" s="34"/>
@@ -39927,16 +39930,16 @@
       <c r="F19" s="33"/>
       <c r="G19" s="33"/>
       <c r="H19" s="40" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I19" s="56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J19" s="54" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K19" s="57" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L19" s="34"/>
       <c r="M19" s="34"/>
@@ -39959,22 +39962,22 @@
         <v>51</v>
       </c>
       <c r="F20" s="33" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G20" s="33" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H20" s="40" t="s">
         <v>29</v>
       </c>
       <c r="I20" s="56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J20" s="54" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K20" s="57" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L20" s="34"/>
       <c r="M20" s="34"/>
@@ -39997,22 +40000,22 @@
         <v>52</v>
       </c>
       <c r="F21" s="45" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G21" s="45" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H21" s="40" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I21" s="62" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J21" s="54" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K21" s="63" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L21" s="34"/>
       <c r="M21" s="34"/>
@@ -40035,22 +40038,22 @@
         <v>53</v>
       </c>
       <c r="F22" s="33" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G22" s="45" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H22" s="40" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I22" s="62" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J22" s="54" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K22" s="63" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L22" s="34"/>
       <c r="M22" s="34"/>
@@ -40069,26 +40072,26 @@
       <c r="D23" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="52" t="s">
-        <v>54</v>
+      <c r="E23" s="68" t="s">
+        <v>129</v>
       </c>
       <c r="F23" s="33" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="G23" s="33" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H23" s="40" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
-      <c r="I23" s="56" t="s">
-        <v>67</v>
+      <c r="I23" s="83" t="s">
+        <v>131</v>
       </c>
       <c r="J23" s="54" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
-      <c r="K23" s="57" t="s">
-        <v>77</v>
+      <c r="K23" s="84" t="s">
+        <v>132</v>
       </c>
       <c r="L23" s="34"/>
       <c r="M23" s="34"/>
@@ -40099,7 +40102,7 @@
         <v>11</v>
       </c>
       <c r="B24" s="73" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C24" s="51">
         <v>3</v>
@@ -40108,25 +40111,25 @@
         <v>9</v>
       </c>
       <c r="E24" s="52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F24" s="33" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G24" s="33" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H24" s="40" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I24" s="56" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J24" s="54" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K24" s="57" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="L24" s="34"/>
       <c r="M24" s="34"/>
@@ -40146,23 +40149,23 @@
         <v>25</v>
       </c>
       <c r="E25" s="52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F25" s="33"/>
       <c r="G25" s="33" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H25" s="40" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I25" s="74" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="J25" s="54" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K25" s="74" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="L25" s="34"/>
       <c r="M25" s="34"/>
@@ -40182,25 +40185,25 @@
         <v>23</v>
       </c>
       <c r="E26" s="61" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F26" s="33" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G26" s="33" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H26" s="40" t="s">
         <v>29</v>
       </c>
       <c r="I26" s="62" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J26" s="54" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K26" s="63" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="L26" s="34"/>
       <c r="M26" s="34"/>
@@ -40218,16 +40221,16 @@
         <v>32</v>
       </c>
       <c r="E27" s="68" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F27" s="33"/>
       <c r="G27" s="33"/>
       <c r="H27" s="40" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I27" s="65"/>
       <c r="J27" s="67" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="K27" s="66"/>
       <c r="L27" s="34"/>
@@ -40248,25 +40251,25 @@
         <v>24</v>
       </c>
       <c r="E28" s="61" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F28" s="33" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G28" s="33" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H28" s="40" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I28" s="62" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J28" s="54" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="K28" s="63" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L28" s="34"/>
       <c r="M28" s="34"/>
@@ -40290,11 +40293,11 @@
     </row>
     <row r="30" spans="1:14" s="36" customFormat="1">
       <c r="A30" s="32"/>
-      <c r="B30" s="78" t="s">
-        <v>108</v>
+      <c r="B30" s="75" t="s">
+        <v>104</v>
       </c>
-      <c r="C30" s="79"/>
-      <c r="D30" s="80"/>
+      <c r="C30" s="76"/>
+      <c r="D30" s="77"/>
       <c r="E30" s="40"/>
       <c r="F30" s="33"/>
       <c r="G30" s="33"/>
@@ -40311,7 +40314,7 @@
         <v>16</v>
       </c>
       <c r="B31" s="33" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C31" s="32">
         <v>1</v>
@@ -40320,25 +40323,25 @@
         <v>32</v>
       </c>
       <c r="E31" s="69" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F31" s="33" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G31" s="33" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H31" s="40" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I31" s="69" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="J31" s="70" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K31" s="69" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="L31" s="34"/>
       <c r="M31" s="34"/>
@@ -40349,7 +40352,7 @@
         <v>17</v>
       </c>
       <c r="B32" s="33" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C32" s="32">
         <v>2</v>
@@ -40358,25 +40361,25 @@
         <v>23</v>
       </c>
       <c r="E32" s="71" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F32" s="33" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="G32" s="33" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H32" s="40" t="s">
         <v>29</v>
       </c>
       <c r="I32" s="71" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="J32" s="72" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K32" s="71" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="L32" s="34"/>
       <c r="M32" s="34"/>
@@ -40387,16 +40390,16 @@
         <v>18</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C33" s="32">
         <v>1</v>
       </c>
       <c r="D33" s="33" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E33" s="40" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F33" s="33"/>
       <c r="G33" s="33"/>
@@ -40426,8 +40429,8 @@
     </row>
     <row r="35" spans="1:14" s="36" customFormat="1">
       <c r="A35" s="32"/>
-      <c r="B35" s="81"/>
-      <c r="C35" s="82"/>
+      <c r="B35" s="78"/>
+      <c r="C35" s="79"/>
       <c r="D35" s="33"/>
       <c r="E35" s="40"/>
       <c r="F35" s="33"/>
@@ -41084,6 +41087,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="G10:G12"/>
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="L10:L12"/>
@@ -41100,7 +41104,6 @@
     <mergeCell ref="H10:H12"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="C10:C12"/>
-    <mergeCell ref="G10:G12"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>